<commit_message>
Consulta planilla por empleado, Angel Chacon
</commit_message>
<xml_diff>
--- a/cronograma de actividades07052020 - copia.xlsx
+++ b/cronograma de actividades07052020 - copia.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Geovani\Desktop\h\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Geovani\Desktop\ultima\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -652,40 +652,58 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -696,24 +714,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -998,8 +998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:N70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O46" sqref="O46"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="O59" sqref="O59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1009,30 +1009,30 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="G3" s="32" t="s">
+      <c r="G3" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="32"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
     </row>
     <row r="5" spans="3:14" ht="23.25" x14ac:dyDescent="0.35">
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="33" t="s">
+      <c r="E5" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="37"/>
-      <c r="J5" s="37"/>
-      <c r="K5" s="37"/>
-      <c r="L5" s="37"/>
-      <c r="M5" s="37"/>
-      <c r="N5" s="37"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="35"/>
+      <c r="M5" s="35"/>
+      <c r="N5" s="35"/>
     </row>
     <row r="6" spans="3:14" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="5" t="s">
@@ -1041,24 +1041,24 @@
       <c r="D6" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E6" s="31" t="s">
+      <c r="E6" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31" t="s">
+      <c r="F6" s="37"/>
+      <c r="G6" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="31"/>
-      <c r="I6" s="31" t="s">
+      <c r="H6" s="37"/>
+      <c r="I6" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="31"/>
-      <c r="K6" s="31"/>
-      <c r="L6" s="31" t="s">
+      <c r="J6" s="37"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="M6" s="31"/>
-      <c r="N6" s="31"/>
+      <c r="M6" s="37"/>
+      <c r="N6" s="37"/>
     </row>
     <row r="7" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C7" s="7">
@@ -1067,24 +1067,24 @@
       <c r="D7" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="38">
+      <c r="E7" s="34">
         <v>43909</v>
       </c>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38">
+      <c r="F7" s="34"/>
+      <c r="G7" s="34">
         <v>43909</v>
       </c>
-      <c r="H7" s="39"/>
-      <c r="I7" s="19" t="s">
+      <c r="H7" s="36"/>
+      <c r="I7" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="25">
-        <v>1</v>
-      </c>
-      <c r="M7" s="25"/>
-      <c r="N7" s="25"/>
+      <c r="J7" s="33"/>
+      <c r="K7" s="33"/>
+      <c r="L7" s="30">
+        <v>1</v>
+      </c>
+      <c r="M7" s="30"/>
+      <c r="N7" s="30"/>
     </row>
     <row r="8" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C8" s="7">
@@ -1094,24 +1094,24 @@
       <c r="D8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="22">
         <v>43910</v>
       </c>
-      <c r="F8" s="24"/>
-      <c r="G8" s="23">
+      <c r="F8" s="23"/>
+      <c r="G8" s="22">
         <v>43910</v>
       </c>
-      <c r="H8" s="24"/>
-      <c r="I8" s="19" t="s">
+      <c r="H8" s="23"/>
+      <c r="I8" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="25">
-        <v>1</v>
-      </c>
-      <c r="M8" s="25"/>
-      <c r="N8" s="25"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="33"/>
+      <c r="L8" s="30">
+        <v>1</v>
+      </c>
+      <c r="M8" s="30"/>
+      <c r="N8" s="30"/>
     </row>
     <row r="9" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C9" s="7">
@@ -1120,24 +1120,24 @@
       <c r="D9" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="23">
+      <c r="E9" s="22">
         <v>43915</v>
       </c>
-      <c r="F9" s="24"/>
-      <c r="G9" s="23">
+      <c r="F9" s="23"/>
+      <c r="G9" s="22">
         <v>43915</v>
       </c>
-      <c r="H9" s="24"/>
-      <c r="I9" s="19" t="s">
+      <c r="H9" s="23"/>
+      <c r="I9" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="25">
-        <v>1</v>
-      </c>
-      <c r="M9" s="25"/>
-      <c r="N9" s="25"/>
+      <c r="J9" s="33"/>
+      <c r="K9" s="33"/>
+      <c r="L9" s="30">
+        <v>1</v>
+      </c>
+      <c r="M9" s="30"/>
+      <c r="N9" s="30"/>
     </row>
     <row r="10" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C10" s="7">
@@ -1146,24 +1146,24 @@
       <c r="D10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="23">
+      <c r="E10" s="22">
         <v>43910</v>
       </c>
-      <c r="F10" s="24"/>
-      <c r="G10" s="23">
+      <c r="F10" s="23"/>
+      <c r="G10" s="22">
         <v>43910</v>
       </c>
-      <c r="H10" s="24"/>
-      <c r="I10" s="19" t="s">
+      <c r="H10" s="23"/>
+      <c r="I10" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="25">
-        <v>1</v>
-      </c>
-      <c r="M10" s="25"/>
-      <c r="N10" s="25"/>
+      <c r="J10" s="33"/>
+      <c r="K10" s="33"/>
+      <c r="L10" s="30">
+        <v>1</v>
+      </c>
+      <c r="M10" s="30"/>
+      <c r="N10" s="30"/>
     </row>
     <row r="11" spans="3:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="7">
@@ -1172,16 +1172,16 @@
       <c r="D11" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19"/>
-      <c r="L11" s="25"/>
-      <c r="M11" s="25"/>
-      <c r="N11" s="25"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="33"/>
+      <c r="K11" s="33"/>
+      <c r="L11" s="30"/>
+      <c r="M11" s="30"/>
+      <c r="N11" s="30"/>
     </row>
     <row r="12" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C12" s="7">
@@ -1190,16 +1190,16 @@
       <c r="D12" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="25"/>
-      <c r="M12" s="25"/>
-      <c r="N12" s="25"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="33"/>
+      <c r="K12" s="33"/>
+      <c r="L12" s="30"/>
+      <c r="M12" s="30"/>
+      <c r="N12" s="30"/>
     </row>
     <row r="13" spans="3:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="C13" s="7"/>
@@ -1220,330 +1220,330 @@
       <c r="D14" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="23">
+      <c r="E14" s="22">
         <v>43956</v>
       </c>
-      <c r="F14" s="24"/>
-      <c r="G14" s="23">
+      <c r="F14" s="23"/>
+      <c r="G14" s="22">
         <v>43956</v>
       </c>
-      <c r="H14" s="24"/>
-      <c r="I14" s="19" t="s">
+      <c r="H14" s="23"/>
+      <c r="I14" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="J14" s="19"/>
-      <c r="K14" s="19"/>
-      <c r="L14" s="25">
-        <v>1</v>
-      </c>
-      <c r="M14" s="25"/>
-      <c r="N14" s="25"/>
+      <c r="J14" s="33"/>
+      <c r="K14" s="33"/>
+      <c r="L14" s="30">
+        <v>1</v>
+      </c>
+      <c r="M14" s="30"/>
+      <c r="N14" s="30"/>
     </row>
     <row r="15" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C15" s="7"/>
       <c r="D15" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E15" s="23">
+      <c r="E15" s="22">
         <v>43956</v>
       </c>
-      <c r="F15" s="24"/>
-      <c r="G15" s="23">
+      <c r="F15" s="23"/>
+      <c r="G15" s="22">
         <v>43956</v>
       </c>
-      <c r="H15" s="24"/>
-      <c r="I15" s="19" t="s">
+      <c r="H15" s="23"/>
+      <c r="I15" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="J15" s="19"/>
-      <c r="K15" s="19"/>
-      <c r="L15" s="25">
-        <v>1</v>
-      </c>
-      <c r="M15" s="25"/>
-      <c r="N15" s="25"/>
+      <c r="J15" s="33"/>
+      <c r="K15" s="33"/>
+      <c r="L15" s="30">
+        <v>1</v>
+      </c>
+      <c r="M15" s="30"/>
+      <c r="N15" s="30"/>
     </row>
     <row r="16" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C16" s="7"/>
       <c r="D16" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="E16" s="23">
+      <c r="E16" s="22">
         <v>43957</v>
       </c>
-      <c r="F16" s="24"/>
-      <c r="G16" s="23">
+      <c r="F16" s="23"/>
+      <c r="G16" s="22">
         <v>43957</v>
       </c>
-      <c r="H16" s="24"/>
-      <c r="I16" s="19" t="s">
+      <c r="H16" s="23"/>
+      <c r="I16" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="J16" s="19"/>
-      <c r="K16" s="19"/>
-      <c r="L16" s="25">
+      <c r="J16" s="33"/>
+      <c r="K16" s="33"/>
+      <c r="L16" s="30">
         <v>0.85</v>
       </c>
-      <c r="M16" s="25"/>
-      <c r="N16" s="25"/>
+      <c r="M16" s="30"/>
+      <c r="N16" s="30"/>
     </row>
     <row r="17" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C17" s="7"/>
       <c r="D17" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E17" s="23">
+      <c r="E17" s="22">
         <v>43957</v>
       </c>
-      <c r="F17" s="24"/>
-      <c r="G17" s="23">
+      <c r="F17" s="23"/>
+      <c r="G17" s="22">
         <v>43959</v>
       </c>
-      <c r="H17" s="24"/>
-      <c r="I17" s="26" t="s">
+      <c r="H17" s="23"/>
+      <c r="I17" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="J17" s="27"/>
-      <c r="K17" s="28"/>
-      <c r="L17" s="20">
-        <v>1</v>
-      </c>
-      <c r="M17" s="21"/>
-      <c r="N17" s="22"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="29"/>
+      <c r="L17" s="24">
+        <v>1</v>
+      </c>
+      <c r="M17" s="25"/>
+      <c r="N17" s="26"/>
     </row>
     <row r="18" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C18" s="7"/>
       <c r="D18" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="E18" s="23">
+      <c r="E18" s="22">
         <v>43956</v>
       </c>
-      <c r="F18" s="24"/>
-      <c r="G18" s="23">
+      <c r="F18" s="23"/>
+      <c r="G18" s="22">
         <v>43956</v>
       </c>
-      <c r="H18" s="24"/>
-      <c r="I18" s="19" t="s">
+      <c r="H18" s="23"/>
+      <c r="I18" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="J18" s="19"/>
-      <c r="K18" s="19"/>
-      <c r="L18" s="25">
+      <c r="J18" s="33"/>
+      <c r="K18" s="33"/>
+      <c r="L18" s="30">
         <v>0.95</v>
       </c>
-      <c r="M18" s="25"/>
-      <c r="N18" s="25"/>
+      <c r="M18" s="30"/>
+      <c r="N18" s="30"/>
     </row>
     <row r="19" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C19" s="7"/>
       <c r="D19" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="E19" s="23">
+      <c r="E19" s="22">
         <v>43956</v>
       </c>
-      <c r="F19" s="24"/>
-      <c r="G19" s="23">
+      <c r="F19" s="23"/>
+      <c r="G19" s="22">
         <v>43956</v>
       </c>
-      <c r="H19" s="24"/>
-      <c r="I19" s="26" t="s">
+      <c r="H19" s="23"/>
+      <c r="I19" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="J19" s="27"/>
-      <c r="K19" s="28"/>
-      <c r="L19" s="25">
+      <c r="J19" s="28"/>
+      <c r="K19" s="29"/>
+      <c r="L19" s="30">
         <v>0.95</v>
       </c>
-      <c r="M19" s="25"/>
-      <c r="N19" s="25"/>
+      <c r="M19" s="30"/>
+      <c r="N19" s="30"/>
     </row>
     <row r="20" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C20" s="7"/>
       <c r="D20" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="E20" s="23">
+      <c r="E20" s="22">
         <v>43957</v>
       </c>
-      <c r="F20" s="24"/>
-      <c r="G20" s="23">
+      <c r="F20" s="23"/>
+      <c r="G20" s="22">
         <v>43957</v>
       </c>
-      <c r="H20" s="24"/>
-      <c r="I20" s="26" t="s">
+      <c r="H20" s="23"/>
+      <c r="I20" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="J20" s="27"/>
-      <c r="K20" s="28"/>
-      <c r="L20" s="25">
+      <c r="J20" s="28"/>
+      <c r="K20" s="29"/>
+      <c r="L20" s="30">
         <v>0.95</v>
       </c>
-      <c r="M20" s="25"/>
-      <c r="N20" s="25"/>
+      <c r="M20" s="30"/>
+      <c r="N20" s="30"/>
     </row>
     <row r="21" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C21" s="7"/>
       <c r="D21" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="E21" s="23">
+      <c r="E21" s="22">
         <v>43957</v>
       </c>
-      <c r="F21" s="24"/>
-      <c r="G21" s="23">
+      <c r="F21" s="23"/>
+      <c r="G21" s="22">
         <v>43959</v>
       </c>
-      <c r="H21" s="24"/>
-      <c r="I21" s="19" t="s">
+      <c r="H21" s="23"/>
+      <c r="I21" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="J21" s="19"/>
-      <c r="K21" s="19"/>
-      <c r="L21" s="20">
+      <c r="J21" s="33"/>
+      <c r="K21" s="33"/>
+      <c r="L21" s="24">
         <v>0.95</v>
       </c>
-      <c r="M21" s="21"/>
-      <c r="N21" s="22"/>
+      <c r="M21" s="25"/>
+      <c r="N21" s="26"/>
     </row>
     <row r="22" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C22" s="7"/>
       <c r="D22" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="E22" s="23">
+      <c r="E22" s="22">
         <v>43956</v>
       </c>
-      <c r="F22" s="24"/>
-      <c r="G22" s="23">
+      <c r="F22" s="23"/>
+      <c r="G22" s="22">
         <v>43956</v>
       </c>
-      <c r="H22" s="24"/>
-      <c r="I22" s="26" t="s">
+      <c r="H22" s="23"/>
+      <c r="I22" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="J22" s="27"/>
-      <c r="K22" s="28"/>
-      <c r="L22" s="25">
+      <c r="J22" s="28"/>
+      <c r="K22" s="29"/>
+      <c r="L22" s="30">
         <v>0.95</v>
       </c>
-      <c r="M22" s="25"/>
-      <c r="N22" s="25"/>
+      <c r="M22" s="30"/>
+      <c r="N22" s="30"/>
     </row>
     <row r="23" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C23" s="7"/>
       <c r="D23" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="E23" s="29">
+      <c r="E23" s="31">
         <v>43956</v>
       </c>
-      <c r="F23" s="30"/>
-      <c r="G23" s="29">
+      <c r="F23" s="32"/>
+      <c r="G23" s="31">
         <v>43956</v>
       </c>
-      <c r="H23" s="30"/>
-      <c r="I23" s="26" t="s">
+      <c r="H23" s="32"/>
+      <c r="I23" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="J23" s="27"/>
-      <c r="K23" s="28"/>
-      <c r="L23" s="25">
+      <c r="J23" s="28"/>
+      <c r="K23" s="29"/>
+      <c r="L23" s="30">
         <v>0.95</v>
       </c>
-      <c r="M23" s="25"/>
-      <c r="N23" s="25"/>
+      <c r="M23" s="30"/>
+      <c r="N23" s="30"/>
     </row>
     <row r="24" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C24" s="7"/>
       <c r="D24" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="E24" s="29">
+      <c r="E24" s="31">
         <v>43957</v>
       </c>
-      <c r="F24" s="30"/>
-      <c r="G24" s="29">
+      <c r="F24" s="32"/>
+      <c r="G24" s="31">
         <v>43957</v>
       </c>
-      <c r="H24" s="30"/>
-      <c r="I24" s="26" t="s">
+      <c r="H24" s="32"/>
+      <c r="I24" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="J24" s="27"/>
-      <c r="K24" s="28"/>
-      <c r="L24" s="25">
+      <c r="J24" s="28"/>
+      <c r="K24" s="29"/>
+      <c r="L24" s="30">
         <v>0.95</v>
       </c>
-      <c r="M24" s="25"/>
-      <c r="N24" s="25"/>
+      <c r="M24" s="30"/>
+      <c r="N24" s="30"/>
     </row>
     <row r="25" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C25" s="7"/>
       <c r="D25" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="E25" s="29">
+      <c r="E25" s="31">
         <v>43957</v>
       </c>
-      <c r="F25" s="30"/>
-      <c r="G25" s="29">
+      <c r="F25" s="32"/>
+      <c r="G25" s="31">
         <v>43959</v>
       </c>
-      <c r="H25" s="30"/>
-      <c r="I25" s="19" t="s">
+      <c r="H25" s="32"/>
+      <c r="I25" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="J25" s="19"/>
-      <c r="K25" s="19"/>
-      <c r="L25" s="20">
+      <c r="J25" s="33"/>
+      <c r="K25" s="33"/>
+      <c r="L25" s="24">
         <v>0.95</v>
       </c>
-      <c r="M25" s="21"/>
-      <c r="N25" s="22"/>
+      <c r="M25" s="25"/>
+      <c r="N25" s="26"/>
     </row>
     <row r="26" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C26" s="7"/>
       <c r="D26" s="8"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="30"/>
-      <c r="G26" s="29"/>
-      <c r="H26" s="30"/>
-      <c r="I26" s="34"/>
-      <c r="J26" s="35"/>
-      <c r="K26" s="36"/>
-      <c r="L26" s="26"/>
-      <c r="M26" s="27"/>
-      <c r="N26" s="28"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="31"/>
+      <c r="H26" s="32"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="21"/>
+      <c r="L26" s="27"/>
+      <c r="M26" s="28"/>
+      <c r="N26" s="29"/>
     </row>
     <row r="27" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C27" s="7"/>
       <c r="D27" s="8"/>
-      <c r="E27" s="29"/>
-      <c r="F27" s="30"/>
-      <c r="G27" s="29"/>
-      <c r="H27" s="30"/>
-      <c r="I27" s="26"/>
-      <c r="J27" s="27"/>
-      <c r="K27" s="28"/>
-      <c r="L27" s="26"/>
-      <c r="M27" s="27"/>
-      <c r="N27" s="28"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="32"/>
+      <c r="I27" s="27"/>
+      <c r="J27" s="28"/>
+      <c r="K27" s="29"/>
+      <c r="L27" s="27"/>
+      <c r="M27" s="28"/>
+      <c r="N27" s="29"/>
     </row>
     <row r="28" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C28" s="7"/>
       <c r="D28" s="8"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="23"/>
-      <c r="H28" s="24"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
-      <c r="K28" s="19"/>
-      <c r="L28" s="25"/>
-      <c r="M28" s="25"/>
-      <c r="N28" s="25"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="33"/>
+      <c r="J28" s="33"/>
+      <c r="K28" s="33"/>
+      <c r="L28" s="30"/>
+      <c r="M28" s="30"/>
+      <c r="N28" s="30"/>
     </row>
     <row r="29" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C29" s="7">
@@ -1552,112 +1552,112 @@
       <c r="D29" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E29" s="23"/>
-      <c r="F29" s="23"/>
-      <c r="G29" s="23"/>
-      <c r="H29" s="23"/>
-      <c r="I29" s="19"/>
-      <c r="J29" s="19"/>
-      <c r="K29" s="19"/>
-      <c r="L29" s="25"/>
-      <c r="M29" s="25"/>
-      <c r="N29" s="25"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="22"/>
+      <c r="I29" s="33"/>
+      <c r="J29" s="33"/>
+      <c r="K29" s="33"/>
+      <c r="L29" s="30"/>
+      <c r="M29" s="30"/>
+      <c r="N29" s="30"/>
     </row>
     <row r="30" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C30" s="7"/>
       <c r="D30" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="E30" s="23">
+      <c r="E30" s="22">
         <v>43915</v>
       </c>
-      <c r="F30" s="24"/>
-      <c r="G30" s="23">
+      <c r="F30" s="23"/>
+      <c r="G30" s="22">
         <v>43917</v>
       </c>
-      <c r="H30" s="24"/>
-      <c r="I30" s="19" t="s">
+      <c r="H30" s="23"/>
+      <c r="I30" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="J30" s="19"/>
-      <c r="K30" s="19"/>
-      <c r="L30" s="25">
-        <v>0.9</v>
-      </c>
-      <c r="M30" s="25"/>
-      <c r="N30" s="25"/>
+      <c r="J30" s="33"/>
+      <c r="K30" s="33"/>
+      <c r="L30" s="30">
+        <v>1</v>
+      </c>
+      <c r="M30" s="30"/>
+      <c r="N30" s="30"/>
     </row>
     <row r="31" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C31" s="7"/>
       <c r="D31" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E31" s="23">
+      <c r="E31" s="22">
         <v>43917</v>
       </c>
-      <c r="F31" s="24"/>
-      <c r="G31" s="23">
+      <c r="F31" s="23"/>
+      <c r="G31" s="22">
         <v>43921</v>
       </c>
-      <c r="H31" s="24"/>
-      <c r="I31" s="19" t="s">
+      <c r="H31" s="23"/>
+      <c r="I31" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="J31" s="19"/>
-      <c r="K31" s="19"/>
-      <c r="L31" s="25">
-        <v>1</v>
-      </c>
-      <c r="M31" s="25"/>
-      <c r="N31" s="25"/>
+      <c r="J31" s="33"/>
+      <c r="K31" s="33"/>
+      <c r="L31" s="30">
+        <v>1</v>
+      </c>
+      <c r="M31" s="30"/>
+      <c r="N31" s="30"/>
     </row>
     <row r="32" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C32" s="7"/>
       <c r="D32" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="E32" s="23">
+      <c r="E32" s="22">
         <v>43918</v>
       </c>
-      <c r="F32" s="24"/>
-      <c r="G32" s="23">
+      <c r="F32" s="23"/>
+      <c r="G32" s="22">
         <v>43922</v>
       </c>
-      <c r="H32" s="24"/>
-      <c r="I32" s="19" t="s">
+      <c r="H32" s="23"/>
+      <c r="I32" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="J32" s="19"/>
-      <c r="K32" s="19"/>
-      <c r="L32" s="20">
-        <v>0.7</v>
-      </c>
-      <c r="M32" s="21"/>
-      <c r="N32" s="22"/>
+      <c r="J32" s="33"/>
+      <c r="K32" s="33"/>
+      <c r="L32" s="24">
+        <v>1</v>
+      </c>
+      <c r="M32" s="25"/>
+      <c r="N32" s="26"/>
     </row>
     <row r="33" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C33" s="7"/>
       <c r="D33" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E33" s="23">
+      <c r="E33" s="22">
         <v>43918</v>
       </c>
-      <c r="F33" s="24"/>
-      <c r="G33" s="23">
+      <c r="F33" s="23"/>
+      <c r="G33" s="22">
         <v>43961</v>
       </c>
-      <c r="H33" s="24"/>
-      <c r="I33" s="19" t="s">
+      <c r="H33" s="23"/>
+      <c r="I33" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="J33" s="19"/>
-      <c r="K33" s="19"/>
-      <c r="L33" s="25">
-        <v>0.7</v>
-      </c>
-      <c r="M33" s="25"/>
-      <c r="N33" s="25"/>
+      <c r="J33" s="33"/>
+      <c r="K33" s="33"/>
+      <c r="L33" s="30">
+        <v>0.95</v>
+      </c>
+      <c r="M33" s="30"/>
+      <c r="N33" s="30"/>
     </row>
     <row r="34" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C34" s="7">
@@ -1666,208 +1666,208 @@
       <c r="D34" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E34" s="23"/>
-      <c r="F34" s="24"/>
-      <c r="G34" s="23"/>
-      <c r="H34" s="24"/>
-      <c r="I34" s="19"/>
-      <c r="J34" s="19"/>
-      <c r="K34" s="19"/>
-      <c r="L34" s="25"/>
-      <c r="M34" s="25"/>
-      <c r="N34" s="25"/>
+      <c r="E34" s="22"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="23"/>
+      <c r="I34" s="33"/>
+      <c r="J34" s="33"/>
+      <c r="K34" s="33"/>
+      <c r="L34" s="30"/>
+      <c r="M34" s="30"/>
+      <c r="N34" s="30"/>
     </row>
     <row r="35" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C35" s="7"/>
       <c r="D35" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="E35" s="23">
+      <c r="E35" s="22">
         <v>43957</v>
       </c>
-      <c r="F35" s="24"/>
-      <c r="G35" s="23">
+      <c r="F35" s="23"/>
+      <c r="G35" s="22">
         <v>43960</v>
       </c>
-      <c r="H35" s="24"/>
-      <c r="I35" s="19" t="s">
+      <c r="H35" s="23"/>
+      <c r="I35" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="J35" s="19"/>
-      <c r="K35" s="19"/>
-      <c r="L35" s="25">
-        <v>1</v>
-      </c>
-      <c r="M35" s="25"/>
-      <c r="N35" s="25"/>
+      <c r="J35" s="33"/>
+      <c r="K35" s="33"/>
+      <c r="L35" s="30">
+        <v>1</v>
+      </c>
+      <c r="M35" s="30"/>
+      <c r="N35" s="30"/>
     </row>
     <row r="36" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C36" s="7"/>
       <c r="D36" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="E36" s="23">
+      <c r="E36" s="22">
         <v>43958</v>
       </c>
-      <c r="F36" s="24"/>
-      <c r="G36" s="23">
+      <c r="F36" s="23"/>
+      <c r="G36" s="22">
         <v>43961</v>
       </c>
-      <c r="H36" s="24"/>
-      <c r="I36" s="19" t="s">
+      <c r="H36" s="23"/>
+      <c r="I36" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="J36" s="19"/>
-      <c r="K36" s="19"/>
-      <c r="L36" s="25">
-        <v>1</v>
-      </c>
-      <c r="M36" s="25"/>
-      <c r="N36" s="25"/>
+      <c r="J36" s="33"/>
+      <c r="K36" s="33"/>
+      <c r="L36" s="30">
+        <v>1</v>
+      </c>
+      <c r="M36" s="30"/>
+      <c r="N36" s="30"/>
     </row>
     <row r="37" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C37" s="7"/>
       <c r="D37" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E37" s="23">
+      <c r="E37" s="22">
         <v>43958</v>
       </c>
-      <c r="F37" s="24"/>
-      <c r="G37" s="23">
+      <c r="F37" s="23"/>
+      <c r="G37" s="22">
         <v>43961</v>
       </c>
-      <c r="H37" s="24"/>
-      <c r="I37" s="19" t="s">
+      <c r="H37" s="23"/>
+      <c r="I37" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="J37" s="19"/>
-      <c r="K37" s="19"/>
-      <c r="L37" s="20">
-        <v>1</v>
-      </c>
-      <c r="M37" s="21"/>
-      <c r="N37" s="22"/>
+      <c r="J37" s="33"/>
+      <c r="K37" s="33"/>
+      <c r="L37" s="24">
+        <v>1</v>
+      </c>
+      <c r="M37" s="25"/>
+      <c r="N37" s="26"/>
     </row>
     <row r="38" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C38" s="7"/>
       <c r="D38" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E38" s="23">
+      <c r="E38" s="22">
         <v>43959</v>
       </c>
-      <c r="F38" s="24"/>
-      <c r="G38" s="23">
+      <c r="F38" s="23"/>
+      <c r="G38" s="22">
         <v>43962</v>
       </c>
-      <c r="H38" s="24"/>
-      <c r="I38" s="19" t="s">
+      <c r="H38" s="23"/>
+      <c r="I38" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="J38" s="19"/>
-      <c r="K38" s="19"/>
-      <c r="L38" s="25">
-        <v>0.75</v>
-      </c>
-      <c r="M38" s="25"/>
-      <c r="N38" s="25"/>
+      <c r="J38" s="33"/>
+      <c r="K38" s="33"/>
+      <c r="L38" s="30">
+        <v>1</v>
+      </c>
+      <c r="M38" s="30"/>
+      <c r="N38" s="30"/>
     </row>
     <row r="39" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C39" s="7"/>
       <c r="D39" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="E39" s="23">
+      <c r="E39" s="22">
         <v>43959</v>
       </c>
-      <c r="F39" s="24"/>
-      <c r="G39" s="23">
+      <c r="F39" s="23"/>
+      <c r="G39" s="22">
         <v>43961</v>
       </c>
-      <c r="H39" s="24"/>
-      <c r="I39" s="19" t="s">
+      <c r="H39" s="23"/>
+      <c r="I39" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="J39" s="19"/>
-      <c r="K39" s="19"/>
-      <c r="L39" s="20">
+      <c r="J39" s="33"/>
+      <c r="K39" s="33"/>
+      <c r="L39" s="24">
         <v>0.8</v>
       </c>
-      <c r="M39" s="21"/>
-      <c r="N39" s="22"/>
+      <c r="M39" s="25"/>
+      <c r="N39" s="26"/>
     </row>
     <row r="40" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C40" s="7"/>
       <c r="D40" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E40" s="23">
+      <c r="E40" s="22">
         <v>43960</v>
       </c>
-      <c r="F40" s="24"/>
-      <c r="G40" s="23">
+      <c r="F40" s="23"/>
+      <c r="G40" s="22">
         <v>43962</v>
       </c>
-      <c r="H40" s="24"/>
-      <c r="I40" s="19" t="s">
+      <c r="H40" s="23"/>
+      <c r="I40" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="J40" s="19"/>
-      <c r="K40" s="19"/>
-      <c r="L40" s="25">
-        <v>0.6</v>
-      </c>
-      <c r="M40" s="25"/>
-      <c r="N40" s="25"/>
+      <c r="J40" s="33"/>
+      <c r="K40" s="33"/>
+      <c r="L40" s="30">
+        <v>0.9</v>
+      </c>
+      <c r="M40" s="30"/>
+      <c r="N40" s="30"/>
     </row>
     <row r="41" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C41" s="7"/>
       <c r="D41" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="E41" s="23">
+      <c r="E41" s="22">
         <v>43960</v>
       </c>
-      <c r="F41" s="24"/>
-      <c r="G41" s="23">
+      <c r="F41" s="23"/>
+      <c r="G41" s="22">
         <v>43960</v>
       </c>
-      <c r="H41" s="24"/>
-      <c r="I41" s="19" t="s">
+      <c r="H41" s="23"/>
+      <c r="I41" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="J41" s="19"/>
-      <c r="K41" s="19"/>
-      <c r="L41" s="20">
-        <v>0.75</v>
-      </c>
-      <c r="M41" s="21"/>
-      <c r="N41" s="22"/>
+      <c r="J41" s="33"/>
+      <c r="K41" s="33"/>
+      <c r="L41" s="24">
+        <v>1</v>
+      </c>
+      <c r="M41" s="25"/>
+      <c r="N41" s="26"/>
     </row>
     <row r="42" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C42" s="7"/>
       <c r="D42" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="E42" s="23">
+      <c r="E42" s="22">
         <v>43961</v>
       </c>
-      <c r="F42" s="24"/>
-      <c r="G42" s="23">
+      <c r="F42" s="23"/>
+      <c r="G42" s="22">
         <v>43961</v>
       </c>
-      <c r="H42" s="24"/>
-      <c r="I42" s="19" t="s">
+      <c r="H42" s="23"/>
+      <c r="I42" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="J42" s="19"/>
-      <c r="K42" s="19"/>
-      <c r="L42" s="25">
-        <v>0.75</v>
-      </c>
-      <c r="M42" s="25"/>
-      <c r="N42" s="25"/>
+      <c r="J42" s="33"/>
+      <c r="K42" s="33"/>
+      <c r="L42" s="30">
+        <v>1</v>
+      </c>
+      <c r="M42" s="30"/>
+      <c r="N42" s="30"/>
     </row>
     <row r="43" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C43" s="7">
@@ -1876,146 +1876,146 @@
       <c r="D43" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="E43" s="23"/>
-      <c r="F43" s="23"/>
-      <c r="G43" s="23"/>
-      <c r="H43" s="23"/>
-      <c r="I43" s="19"/>
-      <c r="J43" s="19"/>
-      <c r="K43" s="19"/>
-      <c r="L43" s="25"/>
-      <c r="M43" s="25"/>
-      <c r="N43" s="25"/>
+      <c r="E43" s="22"/>
+      <c r="F43" s="22"/>
+      <c r="G43" s="22"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="33"/>
+      <c r="J43" s="33"/>
+      <c r="K43" s="33"/>
+      <c r="L43" s="30"/>
+      <c r="M43" s="30"/>
+      <c r="N43" s="30"/>
     </row>
     <row r="44" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C44" s="7"/>
       <c r="D44" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="E44" s="23">
+      <c r="E44" s="22">
         <v>43915</v>
       </c>
-      <c r="F44" s="24"/>
-      <c r="G44" s="23">
+      <c r="F44" s="23"/>
+      <c r="G44" s="22">
         <v>43917</v>
       </c>
-      <c r="H44" s="24"/>
-      <c r="I44" s="19" t="s">
+      <c r="H44" s="23"/>
+      <c r="I44" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="J44" s="19"/>
-      <c r="K44" s="19"/>
-      <c r="L44" s="25">
-        <v>0.75</v>
-      </c>
-      <c r="M44" s="25"/>
-      <c r="N44" s="25"/>
+      <c r="J44" s="33"/>
+      <c r="K44" s="33"/>
+      <c r="L44" s="30">
+        <v>1</v>
+      </c>
+      <c r="M44" s="30"/>
+      <c r="N44" s="30"/>
     </row>
     <row r="45" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C45" s="7"/>
       <c r="D45" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E45" s="23">
+      <c r="E45" s="22">
         <v>43917</v>
       </c>
-      <c r="F45" s="24"/>
-      <c r="G45" s="23">
+      <c r="F45" s="23"/>
+      <c r="G45" s="22">
         <v>43921</v>
       </c>
-      <c r="H45" s="24"/>
-      <c r="I45" s="19" t="s">
+      <c r="H45" s="23"/>
+      <c r="I45" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="J45" s="19"/>
-      <c r="K45" s="19"/>
-      <c r="L45" s="25">
-        <v>0.75</v>
-      </c>
-      <c r="M45" s="25"/>
-      <c r="N45" s="25"/>
+      <c r="J45" s="33"/>
+      <c r="K45" s="33"/>
+      <c r="L45" s="30">
+        <v>1</v>
+      </c>
+      <c r="M45" s="30"/>
+      <c r="N45" s="30"/>
     </row>
     <row r="46" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C46" s="7"/>
       <c r="D46" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E46" s="29">
+      <c r="E46" s="31">
         <v>43960</v>
       </c>
-      <c r="F46" s="30"/>
-      <c r="G46" s="29">
+      <c r="F46" s="32"/>
+      <c r="G46" s="31">
         <v>43931</v>
       </c>
-      <c r="H46" s="30"/>
-      <c r="I46" s="26" t="s">
+      <c r="H46" s="32"/>
+      <c r="I46" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="J46" s="27"/>
-      <c r="K46" s="28"/>
-      <c r="L46" s="20">
-        <v>0.73</v>
-      </c>
-      <c r="M46" s="21"/>
-      <c r="N46" s="22"/>
+      <c r="J46" s="28"/>
+      <c r="K46" s="29"/>
+      <c r="L46" s="24">
+        <v>0.9</v>
+      </c>
+      <c r="M46" s="25"/>
+      <c r="N46" s="26"/>
     </row>
     <row r="47" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C47" s="7"/>
       <c r="D47" s="8"/>
-      <c r="E47" s="23"/>
-      <c r="F47" s="23"/>
-      <c r="G47" s="29"/>
-      <c r="H47" s="30"/>
-      <c r="I47" s="26"/>
-      <c r="J47" s="27"/>
-      <c r="K47" s="28"/>
-      <c r="L47" s="20"/>
-      <c r="M47" s="21"/>
-      <c r="N47" s="22"/>
+      <c r="E47" s="22"/>
+      <c r="F47" s="22"/>
+      <c r="G47" s="31"/>
+      <c r="H47" s="32"/>
+      <c r="I47" s="27"/>
+      <c r="J47" s="28"/>
+      <c r="K47" s="29"/>
+      <c r="L47" s="24"/>
+      <c r="M47" s="25"/>
+      <c r="N47" s="26"/>
     </row>
     <row r="48" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C48" s="7"/>
       <c r="D48" s="3"/>
-      <c r="E48" s="34"/>
-      <c r="F48" s="36"/>
-      <c r="G48" s="34"/>
-      <c r="H48" s="36"/>
-      <c r="I48" s="34"/>
-      <c r="J48" s="35"/>
-      <c r="K48" s="36"/>
-      <c r="L48" s="34"/>
-      <c r="M48" s="35"/>
-      <c r="N48" s="36"/>
+      <c r="E48" s="19"/>
+      <c r="F48" s="21"/>
+      <c r="G48" s="19"/>
+      <c r="H48" s="21"/>
+      <c r="I48" s="19"/>
+      <c r="J48" s="20"/>
+      <c r="K48" s="21"/>
+      <c r="L48" s="19"/>
+      <c r="M48" s="20"/>
+      <c r="N48" s="21"/>
     </row>
     <row r="49" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C49" s="7"/>
       <c r="D49" s="8"/>
-      <c r="E49" s="29"/>
-      <c r="F49" s="30"/>
-      <c r="G49" s="29"/>
-      <c r="H49" s="30"/>
-      <c r="I49" s="26"/>
-      <c r="J49" s="27"/>
-      <c r="K49" s="28"/>
-      <c r="L49" s="20"/>
-      <c r="M49" s="21"/>
-      <c r="N49" s="22"/>
+      <c r="E49" s="31"/>
+      <c r="F49" s="32"/>
+      <c r="G49" s="31"/>
+      <c r="H49" s="32"/>
+      <c r="I49" s="27"/>
+      <c r="J49" s="28"/>
+      <c r="K49" s="29"/>
+      <c r="L49" s="24"/>
+      <c r="M49" s="25"/>
+      <c r="N49" s="26"/>
     </row>
     <row r="50" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C50" s="7"/>
       <c r="D50" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="E50" s="23"/>
-      <c r="F50" s="24"/>
-      <c r="G50" s="23"/>
-      <c r="H50" s="24"/>
-      <c r="I50" s="19"/>
-      <c r="J50" s="19"/>
-      <c r="K50" s="19"/>
-      <c r="L50" s="25"/>
-      <c r="M50" s="25"/>
-      <c r="N50" s="25"/>
+      <c r="E50" s="22"/>
+      <c r="F50" s="23"/>
+      <c r="G50" s="22"/>
+      <c r="H50" s="23"/>
+      <c r="I50" s="33"/>
+      <c r="J50" s="33"/>
+      <c r="K50" s="33"/>
+      <c r="L50" s="30"/>
+      <c r="M50" s="30"/>
+      <c r="N50" s="30"/>
     </row>
     <row r="51" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C51" s="7">
@@ -2024,20 +2024,20 @@
       <c r="D51" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="E51" s="29">
+      <c r="E51" s="31">
         <v>43961</v>
       </c>
-      <c r="F51" s="30"/>
-      <c r="G51" s="29">
+      <c r="F51" s="32"/>
+      <c r="G51" s="31">
         <v>43966</v>
       </c>
-      <c r="H51" s="30"/>
-      <c r="I51" s="26"/>
-      <c r="J51" s="27"/>
-      <c r="K51" s="28"/>
-      <c r="L51" s="20"/>
-      <c r="M51" s="21"/>
-      <c r="N51" s="22"/>
+      <c r="H51" s="32"/>
+      <c r="I51" s="27"/>
+      <c r="J51" s="28"/>
+      <c r="K51" s="29"/>
+      <c r="L51" s="24"/>
+      <c r="M51" s="25"/>
+      <c r="N51" s="26"/>
     </row>
     <row r="52" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C52" s="7">
@@ -2046,24 +2046,24 @@
       <c r="D52" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="E52" s="29">
+      <c r="E52" s="31">
         <v>43952</v>
       </c>
-      <c r="F52" s="30"/>
-      <c r="G52" s="29">
+      <c r="F52" s="32"/>
+      <c r="G52" s="31">
         <v>43967</v>
       </c>
-      <c r="H52" s="30"/>
-      <c r="I52" s="26" t="s">
+      <c r="H52" s="32"/>
+      <c r="I52" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="J52" s="27"/>
-      <c r="K52" s="28"/>
-      <c r="L52" s="20">
-        <v>1</v>
-      </c>
-      <c r="M52" s="21"/>
-      <c r="N52" s="22"/>
+      <c r="J52" s="28"/>
+      <c r="K52" s="29"/>
+      <c r="L52" s="24">
+        <v>1</v>
+      </c>
+      <c r="M52" s="25"/>
+      <c r="N52" s="26"/>
     </row>
     <row r="53" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C53" s="7">
@@ -2072,24 +2072,24 @@
       <c r="D53" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E53" s="29">
+      <c r="E53" s="31">
         <v>43952</v>
       </c>
-      <c r="F53" s="30"/>
-      <c r="G53" s="29">
+      <c r="F53" s="32"/>
+      <c r="G53" s="31">
         <v>43968</v>
       </c>
-      <c r="H53" s="30"/>
-      <c r="I53" s="26" t="s">
+      <c r="H53" s="32"/>
+      <c r="I53" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="J53" s="27"/>
-      <c r="K53" s="28"/>
-      <c r="L53" s="20">
-        <v>1</v>
-      </c>
-      <c r="M53" s="21"/>
-      <c r="N53" s="22"/>
+      <c r="J53" s="28"/>
+      <c r="K53" s="29"/>
+      <c r="L53" s="24">
+        <v>1</v>
+      </c>
+      <c r="M53" s="25"/>
+      <c r="N53" s="26"/>
     </row>
     <row r="54" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C54" s="7">
@@ -2098,24 +2098,24 @@
       <c r="D54" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E54" s="29">
+      <c r="E54" s="31">
         <v>43952</v>
       </c>
-      <c r="F54" s="30"/>
-      <c r="G54" s="29">
+      <c r="F54" s="32"/>
+      <c r="G54" s="31">
         <v>43969</v>
       </c>
-      <c r="H54" s="30"/>
-      <c r="I54" s="26" t="s">
+      <c r="H54" s="32"/>
+      <c r="I54" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="J54" s="27"/>
-      <c r="K54" s="28"/>
-      <c r="L54" s="20">
-        <v>1</v>
-      </c>
-      <c r="M54" s="21"/>
-      <c r="N54" s="22"/>
+      <c r="J54" s="28"/>
+      <c r="K54" s="29"/>
+      <c r="L54" s="24">
+        <v>1</v>
+      </c>
+      <c r="M54" s="25"/>
+      <c r="N54" s="26"/>
     </row>
     <row r="55" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C55" s="7">
@@ -2124,24 +2124,24 @@
       <c r="D55" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E55" s="29">
+      <c r="E55" s="31">
         <v>43952</v>
       </c>
-      <c r="F55" s="30"/>
-      <c r="G55" s="29">
+      <c r="F55" s="32"/>
+      <c r="G55" s="31">
         <v>43970</v>
       </c>
-      <c r="H55" s="30"/>
-      <c r="I55" s="19" t="s">
+      <c r="H55" s="32"/>
+      <c r="I55" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="J55" s="19"/>
-      <c r="K55" s="19"/>
-      <c r="L55" s="25">
-        <v>1</v>
-      </c>
-      <c r="M55" s="25"/>
-      <c r="N55" s="25"/>
+      <c r="J55" s="33"/>
+      <c r="K55" s="33"/>
+      <c r="L55" s="30">
+        <v>1</v>
+      </c>
+      <c r="M55" s="30"/>
+      <c r="N55" s="30"/>
     </row>
     <row r="56" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C56" s="7">
@@ -2150,24 +2150,24 @@
       <c r="D56" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="E56" s="29">
+      <c r="E56" s="31">
         <v>43966</v>
       </c>
-      <c r="F56" s="30"/>
-      <c r="G56" s="29">
+      <c r="F56" s="32"/>
+      <c r="G56" s="31">
         <v>43971</v>
       </c>
-      <c r="H56" s="30"/>
-      <c r="I56" s="19" t="s">
+      <c r="H56" s="32"/>
+      <c r="I56" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="J56" s="19"/>
-      <c r="K56" s="19"/>
-      <c r="L56" s="25">
-        <v>0.75</v>
-      </c>
-      <c r="M56" s="25"/>
-      <c r="N56" s="25"/>
+      <c r="J56" s="33"/>
+      <c r="K56" s="33"/>
+      <c r="L56" s="30">
+        <v>1</v>
+      </c>
+      <c r="M56" s="30"/>
+      <c r="N56" s="30"/>
     </row>
     <row r="57" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C57" s="7">
@@ -2176,24 +2176,24 @@
       <c r="D57" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E57" s="29">
+      <c r="E57" s="31">
         <v>43967</v>
       </c>
-      <c r="F57" s="30"/>
-      <c r="G57" s="29">
+      <c r="F57" s="32"/>
+      <c r="G57" s="31">
         <v>43972</v>
       </c>
-      <c r="H57" s="30"/>
-      <c r="I57" s="19" t="s">
+      <c r="H57" s="32"/>
+      <c r="I57" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="J57" s="19"/>
-      <c r="K57" s="19"/>
-      <c r="L57" s="25">
-        <v>0.75</v>
-      </c>
-      <c r="M57" s="25"/>
-      <c r="N57" s="25"/>
+      <c r="J57" s="33"/>
+      <c r="K57" s="33"/>
+      <c r="L57" s="30">
+        <v>0.9</v>
+      </c>
+      <c r="M57" s="30"/>
+      <c r="N57" s="30"/>
     </row>
     <row r="58" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C58" s="7">
@@ -2202,24 +2202,24 @@
       <c r="D58" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E58" s="29">
+      <c r="E58" s="31">
         <v>43968</v>
       </c>
-      <c r="F58" s="30"/>
-      <c r="G58" s="29">
+      <c r="F58" s="32"/>
+      <c r="G58" s="31">
         <v>43973</v>
       </c>
-      <c r="H58" s="30"/>
-      <c r="I58" s="19" t="s">
+      <c r="H58" s="32"/>
+      <c r="I58" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="J58" s="19"/>
-      <c r="K58" s="19"/>
-      <c r="L58" s="25">
-        <v>1</v>
-      </c>
-      <c r="M58" s="25"/>
-      <c r="N58" s="25"/>
+      <c r="J58" s="33"/>
+      <c r="K58" s="33"/>
+      <c r="L58" s="30">
+        <v>1</v>
+      </c>
+      <c r="M58" s="30"/>
+      <c r="N58" s="30"/>
     </row>
     <row r="59" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C59" s="7">
@@ -2228,24 +2228,24 @@
       <c r="D59" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="E59" s="29">
+      <c r="E59" s="31">
         <v>43969</v>
       </c>
-      <c r="F59" s="30"/>
-      <c r="G59" s="29">
+      <c r="F59" s="32"/>
+      <c r="G59" s="31">
         <v>43974</v>
       </c>
-      <c r="H59" s="30"/>
-      <c r="I59" s="19" t="s">
+      <c r="H59" s="32"/>
+      <c r="I59" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="J59" s="19"/>
-      <c r="K59" s="19"/>
-      <c r="L59" s="25">
-        <v>0.8</v>
-      </c>
-      <c r="M59" s="25"/>
-      <c r="N59" s="25"/>
+      <c r="J59" s="33"/>
+      <c r="K59" s="33"/>
+      <c r="L59" s="30">
+        <v>1</v>
+      </c>
+      <c r="M59" s="30"/>
+      <c r="N59" s="30"/>
     </row>
     <row r="60" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C60" s="7">
@@ -2254,24 +2254,24 @@
       <c r="D60" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E60" s="29">
+      <c r="E60" s="31">
         <v>43970</v>
       </c>
-      <c r="F60" s="30"/>
-      <c r="G60" s="29">
+      <c r="F60" s="32"/>
+      <c r="G60" s="31">
         <v>43975</v>
       </c>
-      <c r="H60" s="30"/>
-      <c r="I60" s="19" t="s">
+      <c r="H60" s="32"/>
+      <c r="I60" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="J60" s="19"/>
-      <c r="K60" s="19"/>
-      <c r="L60" s="25">
-        <v>0.8</v>
-      </c>
-      <c r="M60" s="25"/>
-      <c r="N60" s="25"/>
+      <c r="J60" s="33"/>
+      <c r="K60" s="33"/>
+      <c r="L60" s="30">
+        <v>0.9</v>
+      </c>
+      <c r="M60" s="30"/>
+      <c r="N60" s="30"/>
     </row>
     <row r="61" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C61" s="7">
@@ -2280,44 +2280,44 @@
       <c r="D61" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E61" s="29">
+      <c r="E61" s="31">
         <v>43971</v>
       </c>
-      <c r="F61" s="30"/>
-      <c r="G61" s="29">
+      <c r="F61" s="32"/>
+      <c r="G61" s="31">
         <v>43976</v>
       </c>
-      <c r="H61" s="30"/>
-      <c r="I61" s="19" t="s">
+      <c r="H61" s="32"/>
+      <c r="I61" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="J61" s="19"/>
-      <c r="K61" s="19"/>
-      <c r="L61" s="25">
-        <v>0.8</v>
-      </c>
-      <c r="M61" s="25"/>
-      <c r="N61" s="25"/>
+      <c r="J61" s="33"/>
+      <c r="K61" s="33"/>
+      <c r="L61" s="30">
+        <v>0.95</v>
+      </c>
+      <c r="M61" s="30"/>
+      <c r="N61" s="30"/>
     </row>
     <row r="62" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C62" s="7"/>
       <c r="D62" s="8"/>
-      <c r="E62" s="24"/>
-      <c r="F62" s="24"/>
-      <c r="G62" s="24"/>
-      <c r="H62" s="24"/>
-      <c r="I62" s="19"/>
-      <c r="J62" s="19"/>
-      <c r="K62" s="19"/>
-      <c r="L62" s="37"/>
-      <c r="M62" s="37"/>
-      <c r="N62" s="37"/>
+      <c r="E62" s="23"/>
+      <c r="F62" s="23"/>
+      <c r="G62" s="23"/>
+      <c r="H62" s="23"/>
+      <c r="I62" s="33"/>
+      <c r="J62" s="33"/>
+      <c r="K62" s="33"/>
+      <c r="L62" s="35"/>
+      <c r="M62" s="35"/>
+      <c r="N62" s="35"/>
     </row>
     <row r="65" spans="4:14" ht="26.25" x14ac:dyDescent="0.4">
       <c r="L65" s="13"/>
       <c r="M65" s="12">
         <f>AVERAGE(L7,L8,L9,L10,L14,L15,L28,L30,L31,L34,L44,L45,L46,L52,L54,L53,L55,L56,L57,L58,L59,L60,L61)</f>
-        <v>0.90619047619047643</v>
+        <v>0.98333333333333328</v>
       </c>
     </row>
     <row r="70" spans="4:14" x14ac:dyDescent="0.25">
@@ -2335,24 +2335,186 @@
     </row>
   </sheetData>
   <mergeCells count="228">
-    <mergeCell ref="L48:N48"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="L17:N17"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="L19:N19"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="I23:K23"/>
-    <mergeCell ref="L22:N22"/>
-    <mergeCell ref="L23:N23"/>
-    <mergeCell ref="L25:N25"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="I41:K41"/>
+    <mergeCell ref="L41:N41"/>
+    <mergeCell ref="I32:K32"/>
+    <mergeCell ref="L32:N32"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="I35:K35"/>
+    <mergeCell ref="L35:N35"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="I37:K37"/>
+    <mergeCell ref="L37:N37"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="L16:N16"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="L20:N20"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="L24:N24"/>
+    <mergeCell ref="I39:K39"/>
+    <mergeCell ref="L39:N39"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="G3:L3"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="L7:N7"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="L15:N15"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="L8:N8"/>
+    <mergeCell ref="L11:N11"/>
+    <mergeCell ref="L12:N12"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="E54:F54"/>
+    <mergeCell ref="G53:H53"/>
+    <mergeCell ref="G54:H54"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G52:H52"/>
+    <mergeCell ref="I52:K52"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="G49:H49"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="G59:H59"/>
+    <mergeCell ref="G60:H60"/>
+    <mergeCell ref="G61:H61"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="L18:N18"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="L55:N55"/>
+    <mergeCell ref="L56:N56"/>
+    <mergeCell ref="L50:N50"/>
+    <mergeCell ref="L29:N29"/>
+    <mergeCell ref="L30:N30"/>
+    <mergeCell ref="L43:N43"/>
+    <mergeCell ref="L44:N44"/>
+    <mergeCell ref="L45:N45"/>
+    <mergeCell ref="L53:N53"/>
+    <mergeCell ref="L54:N54"/>
+    <mergeCell ref="L33:N33"/>
+    <mergeCell ref="I29:K29"/>
+    <mergeCell ref="I31:K31"/>
+    <mergeCell ref="I43:K43"/>
+    <mergeCell ref="L52:N52"/>
+    <mergeCell ref="L46:N46"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I14:K14"/>
+    <mergeCell ref="L14:N14"/>
+    <mergeCell ref="L31:N31"/>
+    <mergeCell ref="L34:N34"/>
+    <mergeCell ref="L47:N47"/>
+    <mergeCell ref="L10:N10"/>
+    <mergeCell ref="I44:K44"/>
+    <mergeCell ref="I45:K45"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="I21:K21"/>
+    <mergeCell ref="I25:K25"/>
+    <mergeCell ref="I27:K27"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="L28:N28"/>
+    <mergeCell ref="I30:K30"/>
+    <mergeCell ref="I34:K34"/>
+    <mergeCell ref="I47:K47"/>
+    <mergeCell ref="I46:K46"/>
+    <mergeCell ref="I50:K50"/>
+    <mergeCell ref="G55:H55"/>
+    <mergeCell ref="G56:H56"/>
+    <mergeCell ref="G57:H57"/>
+    <mergeCell ref="I56:K56"/>
+    <mergeCell ref="I55:K55"/>
+    <mergeCell ref="G50:H50"/>
+    <mergeCell ref="I51:K51"/>
+    <mergeCell ref="L51:N51"/>
+    <mergeCell ref="I62:K62"/>
+    <mergeCell ref="L57:N57"/>
+    <mergeCell ref="L58:N58"/>
+    <mergeCell ref="L59:N59"/>
+    <mergeCell ref="L60:N60"/>
+    <mergeCell ref="L61:N61"/>
+    <mergeCell ref="I58:K58"/>
+    <mergeCell ref="I59:K59"/>
+    <mergeCell ref="I60:K60"/>
+    <mergeCell ref="I57:K57"/>
+    <mergeCell ref="I53:K53"/>
+    <mergeCell ref="I54:K54"/>
+    <mergeCell ref="I61:K61"/>
+    <mergeCell ref="L62:N62"/>
+    <mergeCell ref="G62:H62"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E55:F55"/>
+    <mergeCell ref="E56:F56"/>
+    <mergeCell ref="E57:F57"/>
+    <mergeCell ref="E58:F58"/>
+    <mergeCell ref="E59:F59"/>
+    <mergeCell ref="E60:F60"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="G51:H51"/>
+    <mergeCell ref="G58:H58"/>
+    <mergeCell ref="G7:H7"/>
     <mergeCell ref="E61:F61"/>
     <mergeCell ref="E62:F62"/>
     <mergeCell ref="I49:K49"/>
@@ -2377,192 +2539,30 @@
     <mergeCell ref="E48:F48"/>
     <mergeCell ref="G48:H48"/>
     <mergeCell ref="I48:K48"/>
+    <mergeCell ref="L48:N48"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="L17:N17"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="L19:N19"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="I23:K23"/>
+    <mergeCell ref="L22:N22"/>
+    <mergeCell ref="L23:N23"/>
+    <mergeCell ref="L25:N25"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:H21"/>
     <mergeCell ref="I28:K28"/>
     <mergeCell ref="I33:K33"/>
     <mergeCell ref="I17:K17"/>
     <mergeCell ref="L27:N27"/>
-    <mergeCell ref="G62:H62"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E55:F55"/>
-    <mergeCell ref="E56:F56"/>
-    <mergeCell ref="E57:F57"/>
-    <mergeCell ref="E58:F58"/>
-    <mergeCell ref="E59:F59"/>
-    <mergeCell ref="E60:F60"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E51:F51"/>
-    <mergeCell ref="G51:H51"/>
     <mergeCell ref="L21:N21"/>
     <mergeCell ref="L26:N26"/>
-    <mergeCell ref="I51:K51"/>
-    <mergeCell ref="L51:N51"/>
-    <mergeCell ref="I62:K62"/>
-    <mergeCell ref="L57:N57"/>
-    <mergeCell ref="L58:N58"/>
-    <mergeCell ref="L59:N59"/>
-    <mergeCell ref="L60:N60"/>
-    <mergeCell ref="L61:N61"/>
-    <mergeCell ref="I58:K58"/>
-    <mergeCell ref="I59:K59"/>
-    <mergeCell ref="I60:K60"/>
-    <mergeCell ref="I57:K57"/>
-    <mergeCell ref="I53:K53"/>
-    <mergeCell ref="I54:K54"/>
-    <mergeCell ref="L28:N28"/>
-    <mergeCell ref="I30:K30"/>
-    <mergeCell ref="I34:K34"/>
-    <mergeCell ref="I47:K47"/>
-    <mergeCell ref="I46:K46"/>
-    <mergeCell ref="I50:K50"/>
-    <mergeCell ref="G55:H55"/>
-    <mergeCell ref="G56:H56"/>
-    <mergeCell ref="G57:H57"/>
-    <mergeCell ref="G58:H58"/>
-    <mergeCell ref="I61:K61"/>
-    <mergeCell ref="I56:K56"/>
-    <mergeCell ref="I55:K55"/>
-    <mergeCell ref="L62:N62"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="L14:N14"/>
-    <mergeCell ref="L31:N31"/>
-    <mergeCell ref="L34:N34"/>
-    <mergeCell ref="L47:N47"/>
-    <mergeCell ref="L10:N10"/>
-    <mergeCell ref="I44:K44"/>
-    <mergeCell ref="I45:K45"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="I21:K21"/>
-    <mergeCell ref="I25:K25"/>
-    <mergeCell ref="I27:K27"/>
-    <mergeCell ref="G46:H46"/>
-    <mergeCell ref="G50:H50"/>
-    <mergeCell ref="G59:H59"/>
-    <mergeCell ref="G60:H60"/>
-    <mergeCell ref="G61:H61"/>
-    <mergeCell ref="I18:K18"/>
-    <mergeCell ref="L18:N18"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="L55:N55"/>
-    <mergeCell ref="L56:N56"/>
-    <mergeCell ref="L50:N50"/>
-    <mergeCell ref="L29:N29"/>
-    <mergeCell ref="L30:N30"/>
-    <mergeCell ref="L43:N43"/>
-    <mergeCell ref="L44:N44"/>
-    <mergeCell ref="L45:N45"/>
-    <mergeCell ref="L53:N53"/>
-    <mergeCell ref="L54:N54"/>
-    <mergeCell ref="L33:N33"/>
-    <mergeCell ref="I29:K29"/>
-    <mergeCell ref="I31:K31"/>
-    <mergeCell ref="I43:K43"/>
-    <mergeCell ref="L52:N52"/>
-    <mergeCell ref="L46:N46"/>
-    <mergeCell ref="I26:K26"/>
-    <mergeCell ref="E53:F53"/>
-    <mergeCell ref="E54:F54"/>
-    <mergeCell ref="G53:H53"/>
-    <mergeCell ref="G54:H54"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G52:H52"/>
-    <mergeCell ref="I52:K52"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="G49:H49"/>
-    <mergeCell ref="E52:F52"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="G43:H43"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="L6:N6"/>
-    <mergeCell ref="G3:L3"/>
-    <mergeCell ref="E5:H5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="L7:N7"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="L15:N15"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="I12:K12"/>
-    <mergeCell ref="L8:N8"/>
-    <mergeCell ref="L11:N11"/>
-    <mergeCell ref="L12:N12"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="L5:N5"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="I15:K15"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="L16:N16"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="I20:K20"/>
-    <mergeCell ref="L20:N20"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="L24:N24"/>
-    <mergeCell ref="I39:K39"/>
-    <mergeCell ref="L39:N39"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="G41:H41"/>
-    <mergeCell ref="I41:K41"/>
-    <mergeCell ref="L41:N41"/>
-    <mergeCell ref="I32:K32"/>
-    <mergeCell ref="L32:N32"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="I35:K35"/>
-    <mergeCell ref="L35:N35"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="I37:K37"/>
-    <mergeCell ref="L37:N37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>